<commit_message>
Updated standard documents with phase set directly in the document
</commit_message>
<xml_diff>
--- a/templates/data-1044/StandardDocuments/Gevinstverktøy.xlsx
+++ b/templates/data-1044/StandardDocuments/Gevinstverktøy.xlsx
@@ -22308,4 +22308,200 @@
   <drawing r:id="rId2"/>
   <legacyDrawingHF r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Prosjektdokument" ma:contentTypeID="0x010100293FDE3FCADA480B9A77BBDAD7DFA28C0100860EB8D0A6C41A489350A1AED607DCA8" ma:contentTypeVersion="48" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="e8cce5c97d0f6d1d73b99cec536b5027">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="fcde26a5-0f5e-4ce4-9c4e-5d7667e77a32" xmlns:ns3="6242508b-47dd-4228-87f2-8f4c54fa3af7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb6ba19d300d22229c9e3f2e03597c49" ns1:_="" ns3:_="">
+    <xsd:import namespace="fcde26a5-0f5e-4ce4-9c4e-5d7667e77a32"/>
+    <xsd:import namespace="6242508b-47dd-4228-87f2-8f4c54fa3af7"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns1:j25543a5815d485da9a5e0773ad762e9" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAllLabel" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fcde26a5-0f5e-4ce4-9c4e-5d7667e77a32" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="j25543a5815d485da9a5e0773ad762e9" ma:index="8" nillable="true" ma:taxonomy="true" ma:internalName="j25543a5815d485da9a5e0773ad762e9" ma:taxonomyFieldName="GtProjectPhase" ma:displayName="Fase" ma:indexed="true" ma:default="" ma:fieldId="{325543a5-815d-485d-a9a5-e0773ad762e9}" ma:sspId="a08c65c3-98d0-478f-a073-d98dd80897ac" ma:termSetId="abcfc9d9-a263-4abb-8234-be973c46258a" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6242508b-47dd-4228-87f2-8f4c54fa3af7" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="9" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:description="" ma:hidden="true" ma:list="{7e6ed586-3813-4ab9-91a6-95e7318c1a1f}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="fcde26a5-0f5e-4ce4-9c4e-5d7667e77a32">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAllLabel" ma:index="10" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:description="" ma:hidden="true" ma:list="{7e6ed586-3813-4ab9-91a6-95e7318c1a1f}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="fcde26a5-0f5e-4ce4-9c4e-5d7667e77a32">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="11" ma:displayName="Innholdstype"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Tittel"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <j25543a5815d485da9a5e0773ad762e9 xmlns="fcde26a5-0f5e-4ce4-9c4e-5d7667e77a32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Realisere</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b7ba84f0-70b9-45c4-8c50-8f73bf15bbec</TermId>
+        </TermInfo>
+      </Terms>
+    </j25543a5815d485da9a5e0773ad762e9>
+    <TaxCatchAll xmlns="6242508b-47dd-4228-87f2-8f4c54fa3af7">
+      <Value>12</Value>
+    </TaxCatchAll>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF4040E1-678D-4CC3-B8D9-65909231992D}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C174F13-00F9-4B0D-B228-06F68F017D65}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0E33CA-A5F2-4FA5-B48E-907021753296}"/>
 </file>
</xml_diff>

<commit_message>
Updated standard documents from PVV 3.0
</commit_message>
<xml_diff>
--- a/templates/data-1044/StandardDocuments/Gevinstverktøy.xlsx
+++ b/templates/data-1044/StandardDocuments/Gevinstverktøy.xlsx
@@ -22311,8 +22311,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Prosjektdokument" ma:contentTypeID="0x010100293FDE3FCADA480B9A77BBDAD7DFA28C0100860EB8D0A6C41A489350A1AED607DCA8" ma:contentTypeVersion="48" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="e8cce5c97d0f6d1d73b99cec536b5027">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="fcde26a5-0f5e-4ce4-9c4e-5d7667e77a32" xmlns:ns3="6242508b-47dd-4228-87f2-8f4c54fa3af7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb6ba19d300d22229c9e3f2e03597c49" ns1:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Prosjektdokument" ma:contentTypeID="0x010100293FDE3FCADA480B9A77BBDAD7DFA28C0100860EB8D0A6C41A489350A1AED607DCA8" ma:contentTypeVersion="48" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="f231ac969c83eea93ecd61db62a571e1">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="fcde26a5-0f5e-4ce4-9c4e-5d7667e77a32" xmlns:ns3="6242508b-47dd-4228-87f2-8f4c54fa3af7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e05611011757f6310e51efa0bb5fcb50" ns1:_="" ns3:_="">
     <xsd:import namespace="fcde26a5-0f5e-4ce4-9c4e-5d7667e77a32"/>
     <xsd:import namespace="6242508b-47dd-4228-87f2-8f4c54fa3af7"/>
     <xsd:element name="properties">
@@ -22495,7 +22495,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF4040E1-678D-4CC3-B8D9-65909231992D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB1B4E46-31D4-49CA-B0D3-045EED60CB93}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>